<commit_message>
bumped direct aid mpc
bumped first quarter up from 0.08 to 0.18. Q1 and Q2 became more positive, Q3 more negative
</commit_message>
<xml_diff>
--- a/data/add-ons/add_factors.xlsx
+++ b/data/add-ons/add_factors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malcalakovalski/Documents/Projects/Fiscal-Impact-Measure/data/add-ons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5F2670-DA75-7940-8B0C-49671FEDBFEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352006F7-A6EA-B64A-B9C2-877764618489}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19500" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
   </bookViews>
@@ -3571,21 +3571,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3607,14 +3592,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4130,10 +4130,10 @@
   <dimension ref="A1:AQ120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="M62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="J61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O82" sqref="O82"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14982,68 +14982,68 @@
       <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="356" t="s">
+      <c r="A2" s="351" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="356"/>
-      <c r="C2" s="356"/>
-      <c r="D2" s="356"/>
-      <c r="E2" s="356"/>
-      <c r="F2" s="356"/>
-      <c r="G2" s="356"/>
-      <c r="H2" s="356"/>
-      <c r="I2" s="356"/>
-      <c r="J2" s="356"/>
+      <c r="B2" s="351"/>
+      <c r="C2" s="351"/>
+      <c r="D2" s="351"/>
+      <c r="E2" s="351"/>
+      <c r="F2" s="351"/>
+      <c r="G2" s="351"/>
+      <c r="H2" s="351"/>
+      <c r="I2" s="351"/>
+      <c r="J2" s="351"/>
       <c r="K2" s="77"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="356" t="s">
+      <c r="A3" s="351" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="356"/>
-      <c r="C3" s="356"/>
-      <c r="D3" s="356"/>
-      <c r="E3" s="356"/>
-      <c r="F3" s="356"/>
-      <c r="G3" s="356"/>
-      <c r="H3" s="356"/>
-      <c r="I3" s="356"/>
-      <c r="J3" s="356"/>
+      <c r="B3" s="351"/>
+      <c r="C3" s="351"/>
+      <c r="D3" s="351"/>
+      <c r="E3" s="351"/>
+      <c r="F3" s="351"/>
+      <c r="G3" s="351"/>
+      <c r="H3" s="351"/>
+      <c r="I3" s="351"/>
+      <c r="J3" s="351"/>
       <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="357"/>
-      <c r="B4" s="357"/>
-      <c r="C4" s="357"/>
-      <c r="D4" s="357"/>
-      <c r="E4" s="357"/>
-      <c r="F4" s="357"/>
-      <c r="G4" s="357"/>
-      <c r="H4" s="357"/>
-      <c r="I4" s="357"/>
-      <c r="J4" s="357"/>
-      <c r="K4" s="362" t="s">
+      <c r="A4" s="352"/>
+      <c r="B4" s="352"/>
+      <c r="C4" s="352"/>
+      <c r="D4" s="352"/>
+      <c r="E4" s="352"/>
+      <c r="F4" s="352"/>
+      <c r="G4" s="352"/>
+      <c r="H4" s="352"/>
+      <c r="I4" s="352"/>
+      <c r="J4" s="352"/>
+      <c r="K4" s="357" t="s">
         <v>160</v>
       </c>
-      <c r="L4" s="362"/>
-      <c r="M4" s="362"/>
-      <c r="N4" s="362"/>
+      <c r="L4" s="357"/>
+      <c r="M4" s="357"/>
+      <c r="N4" s="357"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="47"/>
       <c r="B5" s="48"/>
-      <c r="C5" s="358" t="s">
+      <c r="C5" s="353" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="359"/>
-      <c r="E5" s="359"/>
-      <c r="F5" s="359"/>
-      <c r="G5" s="359"/>
-      <c r="H5" s="359"/>
-      <c r="I5" s="359"/>
-      <c r="J5" s="360"/>
+      <c r="D5" s="354"/>
+      <c r="E5" s="354"/>
+      <c r="F5" s="354"/>
+      <c r="G5" s="354"/>
+      <c r="H5" s="354"/>
+      <c r="I5" s="354"/>
+      <c r="J5" s="355"/>
       <c r="K5" s="78"/>
-      <c r="L5" s="361" t="s">
+      <c r="L5" s="356" t="s">
         <v>107</v>
       </c>
       <c r="M5" s="327"/>
@@ -15054,16 +15054,16 @@
         <v>109</v>
       </c>
       <c r="B6" s="49"/>
-      <c r="C6" s="352">
+      <c r="C6" s="359">
         <v>2020</v>
       </c>
-      <c r="D6" s="353"/>
-      <c r="E6" s="353"/>
-      <c r="F6" s="353"/>
-      <c r="G6" s="353"/>
-      <c r="H6" s="353"/>
-      <c r="I6" s="353"/>
-      <c r="J6" s="354"/>
+      <c r="D6" s="360"/>
+      <c r="E6" s="360"/>
+      <c r="F6" s="360"/>
+      <c r="G6" s="360"/>
+      <c r="H6" s="360"/>
+      <c r="I6" s="360"/>
+      <c r="J6" s="361"/>
       <c r="K6" s="78" t="s">
         <v>135</v>
       </c>
@@ -15535,12 +15535,12 @@
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="K23" s="355" t="s">
+      <c r="K23" s="362" t="s">
         <v>108</v>
       </c>
-      <c r="L23" s="355"/>
-      <c r="M23" s="355"/>
-      <c r="N23" s="355"/>
+      <c r="L23" s="362"/>
+      <c r="M23" s="362"/>
+      <c r="N23" s="362"/>
       <c r="O23" s="35" t="s">
         <v>146</v>
       </c>
@@ -15709,7 +15709,7 @@
       <c r="S27" s="72"/>
     </row>
     <row r="28" spans="3:23" x14ac:dyDescent="0.2">
-      <c r="I28" s="351" t="s">
+      <c r="I28" s="358" t="s">
         <v>258</v>
       </c>
       <c r="J28" s="82" t="s">
@@ -15759,7 +15759,7 @@
       <c r="H29">
         <v>67</v>
       </c>
-      <c r="I29" s="351"/>
+      <c r="I29" s="358"/>
       <c r="J29" s="82" t="s">
         <v>143</v>
       </c>
@@ -15807,7 +15807,7 @@
         <f>H29</f>
         <v>67</v>
       </c>
-      <c r="I30" s="351"/>
+      <c r="I30" s="358"/>
       <c r="J30" s="82" t="s">
         <v>142</v>
       </c>
@@ -15855,7 +15855,7 @@
         <f>24</f>
         <v>24</v>
       </c>
-      <c r="I31" s="351"/>
+      <c r="I31" s="358"/>
       <c r="J31" s="35" t="s">
         <v>140</v>
       </c>
@@ -15917,7 +15917,7 @@
         <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="I33" s="351" t="s">
+      <c r="I33" s="358" t="s">
         <v>141</v>
       </c>
       <c r="J33" s="85" t="s">
@@ -15965,7 +15965,7 @@
       </c>
     </row>
     <row r="34" spans="3:23" x14ac:dyDescent="0.2">
-      <c r="I34" s="351"/>
+      <c r="I34" s="358"/>
       <c r="J34" t="s">
         <v>259</v>
       </c>
@@ -16202,12 +16202,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="K4:N4"/>
     <mergeCell ref="O22:R22"/>
     <mergeCell ref="S22:V22"/>
     <mergeCell ref="I28:I31"/>
@@ -16215,6 +16209,12 @@
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="K23:N23"/>
     <mergeCell ref="K22:N22"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="K4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16321,22 +16321,22 @@
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
-      <c r="E6" s="364" t="s">
+      <c r="E6" s="366" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="364"/>
-      <c r="G6" s="364"/>
-      <c r="H6" s="364"/>
-      <c r="I6" s="364"/>
-      <c r="J6" s="364"/>
-      <c r="K6" s="364"/>
-      <c r="L6" s="364"/>
-      <c r="M6" s="364"/>
-      <c r="N6" s="364"/>
-      <c r="O6" s="364"/>
-      <c r="P6" s="364"/>
-      <c r="Q6" s="364"/>
-      <c r="R6" s="364"/>
+      <c r="F6" s="366"/>
+      <c r="G6" s="366"/>
+      <c r="H6" s="366"/>
+      <c r="I6" s="366"/>
+      <c r="J6" s="366"/>
+      <c r="K6" s="366"/>
+      <c r="L6" s="366"/>
+      <c r="M6" s="366"/>
+      <c r="N6" s="366"/>
+      <c r="O6" s="366"/>
+      <c r="P6" s="366"/>
+      <c r="Q6" s="366"/>
+      <c r="R6" s="366"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="363" t="s">
@@ -17072,21 +17072,21 @@
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="365" t="s">
+      <c r="H27" s="364" t="s">
         <v>95</v>
       </c>
-      <c r="I27" s="365"/>
-      <c r="J27" s="365"/>
-      <c r="K27" s="365"/>
-      <c r="L27" s="365"/>
-      <c r="M27" s="365"/>
-      <c r="N27" s="365"/>
-      <c r="O27" s="365"/>
-      <c r="P27" s="365"/>
-      <c r="Q27" s="365"/>
-      <c r="R27" s="365"/>
-      <c r="S27" s="365"/>
-      <c r="T27" s="365"/>
+      <c r="I27" s="364"/>
+      <c r="J27" s="364"/>
+      <c r="K27" s="364"/>
+      <c r="L27" s="364"/>
+      <c r="M27" s="364"/>
+      <c r="N27" s="364"/>
+      <c r="O27" s="364"/>
+      <c r="P27" s="364"/>
+      <c r="Q27" s="364"/>
+      <c r="R27" s="364"/>
+      <c r="S27" s="364"/>
+      <c r="T27" s="364"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
@@ -17402,21 +17402,21 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
-      <c r="F37" s="366" t="s">
+      <c r="F37" s="365" t="s">
         <v>99</v>
       </c>
-      <c r="G37" s="366"/>
-      <c r="H37" s="366"/>
-      <c r="I37" s="366"/>
-      <c r="J37" s="366"/>
-      <c r="K37" s="366"/>
-      <c r="L37" s="366"/>
-      <c r="M37" s="366"/>
-      <c r="N37" s="366"/>
-      <c r="O37" s="366"/>
-      <c r="P37" s="366"/>
-      <c r="Q37" s="366"/>
-      <c r="R37" s="366"/>
+      <c r="G37" s="365"/>
+      <c r="H37" s="365"/>
+      <c r="I37" s="365"/>
+      <c r="J37" s="365"/>
+      <c r="K37" s="365"/>
+      <c r="L37" s="365"/>
+      <c r="M37" s="365"/>
+      <c r="N37" s="365"/>
+      <c r="O37" s="365"/>
+      <c r="P37" s="365"/>
+      <c r="Q37" s="365"/>
+      <c r="R37" s="365"/>
     </row>
     <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="24" t="s">
@@ -17732,21 +17732,21 @@
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
-      <c r="F48" s="365" t="s">
+      <c r="F48" s="364" t="s">
         <v>101</v>
       </c>
-      <c r="G48" s="365"/>
-      <c r="H48" s="365"/>
-      <c r="I48" s="365"/>
-      <c r="J48" s="365"/>
-      <c r="K48" s="365"/>
-      <c r="L48" s="365"/>
-      <c r="M48" s="365"/>
-      <c r="N48" s="365"/>
-      <c r="O48" s="365"/>
-      <c r="P48" s="365"/>
-      <c r="Q48" s="365"/>
-      <c r="R48" s="365"/>
+      <c r="G48" s="364"/>
+      <c r="H48" s="364"/>
+      <c r="I48" s="364"/>
+      <c r="J48" s="364"/>
+      <c r="K48" s="364"/>
+      <c r="L48" s="364"/>
+      <c r="M48" s="364"/>
+      <c r="N48" s="364"/>
+      <c r="O48" s="364"/>
+      <c r="P48" s="364"/>
+      <c r="Q48" s="364"/>
+      <c r="R48" s="364"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
@@ -18058,6 +18058,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E6:R6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="H27:T27"/>
     <mergeCell ref="F37:R37"/>
@@ -18066,12 +18072,6 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E6:R6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -32784,18 +32784,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -33016,6 +33016,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170E13C6-C717-4C73-9EC5-EE5855C1B9D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -33028,14 +33036,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updated education stabilization fund data
</commit_message>
<xml_diff>
--- a/data/add-ons/add_factors.xlsx
+++ b/data/add-ons/add_factors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malcalakovalski/Documents/Projects/Fiscal-Impact-Measure/data/add-ons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352006F7-A6EA-B64A-B9C2-877764618489}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940158F6-1A3C-0145-B760-C46EB79B61AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19500" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
   </bookViews>
@@ -3571,6 +3571,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3592,29 +3607,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4130,10 +4130,10 @@
   <dimension ref="A1:AQ120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="J61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="J60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="N82" sqref="N82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8642,14 +8642,14 @@
       <c r="K72" s="202"/>
       <c r="L72" s="206">
         <f>SUM(L74:L76)</f>
-        <v>87000</v>
+        <v>90400</v>
       </c>
       <c r="M72" s="301">
         <v>97000</v>
       </c>
       <c r="N72" s="308">
         <f>SUM(N74:N76)</f>
-        <v>107000</v>
+        <v>87200</v>
       </c>
       <c r="O72" s="116">
         <f t="shared" ref="O72:Z72" si="45">O73+O77</f>
@@ -8853,13 +8853,13 @@
       <c r="J75" s="202"/>
       <c r="K75" s="202"/>
       <c r="L75" s="202">
-        <v>25000</v>
+        <v>28400</v>
       </c>
       <c r="M75" s="301">
-        <v>25000</v>
+        <v>15800</v>
       </c>
       <c r="N75" s="308">
-        <v>35000</v>
+        <v>15200</v>
       </c>
       <c r="O75" s="116">
         <v>18000</v>
@@ -9308,14 +9308,14 @@
       </c>
       <c r="L82" s="206">
         <f>L70+L72</f>
-        <v>279250</v>
+        <v>282650</v>
       </c>
       <c r="M82" s="301">
         <v>300600</v>
       </c>
       <c r="N82" s="308">
         <f>N70+N72</f>
-        <v>303951</v>
+        <v>284151</v>
       </c>
       <c r="O82" s="144">
         <f t="shared" ref="O82:Z82" si="48">O70+O72</f>
@@ -14982,68 +14982,68 @@
       <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="351" t="s">
+      <c r="A2" s="356" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="351"/>
-      <c r="C2" s="351"/>
-      <c r="D2" s="351"/>
-      <c r="E2" s="351"/>
-      <c r="F2" s="351"/>
-      <c r="G2" s="351"/>
-      <c r="H2" s="351"/>
-      <c r="I2" s="351"/>
-      <c r="J2" s="351"/>
+      <c r="B2" s="356"/>
+      <c r="C2" s="356"/>
+      <c r="D2" s="356"/>
+      <c r="E2" s="356"/>
+      <c r="F2" s="356"/>
+      <c r="G2" s="356"/>
+      <c r="H2" s="356"/>
+      <c r="I2" s="356"/>
+      <c r="J2" s="356"/>
       <c r="K2" s="77"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="351" t="s">
+      <c r="A3" s="356" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="351"/>
-      <c r="C3" s="351"/>
-      <c r="D3" s="351"/>
-      <c r="E3" s="351"/>
-      <c r="F3" s="351"/>
-      <c r="G3" s="351"/>
-      <c r="H3" s="351"/>
-      <c r="I3" s="351"/>
-      <c r="J3" s="351"/>
+      <c r="B3" s="356"/>
+      <c r="C3" s="356"/>
+      <c r="D3" s="356"/>
+      <c r="E3" s="356"/>
+      <c r="F3" s="356"/>
+      <c r="G3" s="356"/>
+      <c r="H3" s="356"/>
+      <c r="I3" s="356"/>
+      <c r="J3" s="356"/>
       <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="352"/>
-      <c r="B4" s="352"/>
-      <c r="C4" s="352"/>
-      <c r="D4" s="352"/>
-      <c r="E4" s="352"/>
-      <c r="F4" s="352"/>
-      <c r="G4" s="352"/>
-      <c r="H4" s="352"/>
-      <c r="I4" s="352"/>
-      <c r="J4" s="352"/>
-      <c r="K4" s="357" t="s">
+      <c r="A4" s="357"/>
+      <c r="B4" s="357"/>
+      <c r="C4" s="357"/>
+      <c r="D4" s="357"/>
+      <c r="E4" s="357"/>
+      <c r="F4" s="357"/>
+      <c r="G4" s="357"/>
+      <c r="H4" s="357"/>
+      <c r="I4" s="357"/>
+      <c r="J4" s="357"/>
+      <c r="K4" s="362" t="s">
         <v>160</v>
       </c>
-      <c r="L4" s="357"/>
-      <c r="M4" s="357"/>
-      <c r="N4" s="357"/>
+      <c r="L4" s="362"/>
+      <c r="M4" s="362"/>
+      <c r="N4" s="362"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="47"/>
       <c r="B5" s="48"/>
-      <c r="C5" s="353" t="s">
+      <c r="C5" s="358" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="354"/>
-      <c r="E5" s="354"/>
-      <c r="F5" s="354"/>
-      <c r="G5" s="354"/>
-      <c r="H5" s="354"/>
-      <c r="I5" s="354"/>
-      <c r="J5" s="355"/>
+      <c r="D5" s="359"/>
+      <c r="E5" s="359"/>
+      <c r="F5" s="359"/>
+      <c r="G5" s="359"/>
+      <c r="H5" s="359"/>
+      <c r="I5" s="359"/>
+      <c r="J5" s="360"/>
       <c r="K5" s="78"/>
-      <c r="L5" s="356" t="s">
+      <c r="L5" s="361" t="s">
         <v>107</v>
       </c>
       <c r="M5" s="327"/>
@@ -15054,16 +15054,16 @@
         <v>109</v>
       </c>
       <c r="B6" s="49"/>
-      <c r="C6" s="359">
+      <c r="C6" s="352">
         <v>2020</v>
       </c>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
-      <c r="H6" s="360"/>
-      <c r="I6" s="360"/>
-      <c r="J6" s="361"/>
+      <c r="D6" s="353"/>
+      <c r="E6" s="353"/>
+      <c r="F6" s="353"/>
+      <c r="G6" s="353"/>
+      <c r="H6" s="353"/>
+      <c r="I6" s="353"/>
+      <c r="J6" s="354"/>
       <c r="K6" s="78" t="s">
         <v>135</v>
       </c>
@@ -15535,12 +15535,12 @@
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="K23" s="362" t="s">
+      <c r="K23" s="355" t="s">
         <v>108</v>
       </c>
-      <c r="L23" s="362"/>
-      <c r="M23" s="362"/>
-      <c r="N23" s="362"/>
+      <c r="L23" s="355"/>
+      <c r="M23" s="355"/>
+      <c r="N23" s="355"/>
       <c r="O23" s="35" t="s">
         <v>146</v>
       </c>
@@ -15709,7 +15709,7 @@
       <c r="S27" s="72"/>
     </row>
     <row r="28" spans="3:23" x14ac:dyDescent="0.2">
-      <c r="I28" s="358" t="s">
+      <c r="I28" s="351" t="s">
         <v>258</v>
       </c>
       <c r="J28" s="82" t="s">
@@ -15759,7 +15759,7 @@
       <c r="H29">
         <v>67</v>
       </c>
-      <c r="I29" s="358"/>
+      <c r="I29" s="351"/>
       <c r="J29" s="82" t="s">
         <v>143</v>
       </c>
@@ -15807,7 +15807,7 @@
         <f>H29</f>
         <v>67</v>
       </c>
-      <c r="I30" s="358"/>
+      <c r="I30" s="351"/>
       <c r="J30" s="82" t="s">
         <v>142</v>
       </c>
@@ -15855,7 +15855,7 @@
         <f>24</f>
         <v>24</v>
       </c>
-      <c r="I31" s="358"/>
+      <c r="I31" s="351"/>
       <c r="J31" s="35" t="s">
         <v>140</v>
       </c>
@@ -15917,7 +15917,7 @@
         <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="I33" s="358" t="s">
+      <c r="I33" s="351" t="s">
         <v>141</v>
       </c>
       <c r="J33" s="85" t="s">
@@ -15965,7 +15965,7 @@
       </c>
     </row>
     <row r="34" spans="3:23" x14ac:dyDescent="0.2">
-      <c r="I34" s="358"/>
+      <c r="I34" s="351"/>
       <c r="J34" t="s">
         <v>259</v>
       </c>
@@ -16202,6 +16202,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="K4:N4"/>
     <mergeCell ref="O22:R22"/>
     <mergeCell ref="S22:V22"/>
     <mergeCell ref="I28:I31"/>
@@ -16209,12 +16215,6 @@
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="K23:N23"/>
     <mergeCell ref="K22:N22"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="K4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16321,22 +16321,22 @@
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
-      <c r="E6" s="366" t="s">
+      <c r="E6" s="364" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="366"/>
-      <c r="G6" s="366"/>
-      <c r="H6" s="366"/>
-      <c r="I6" s="366"/>
-      <c r="J6" s="366"/>
-      <c r="K6" s="366"/>
-      <c r="L6" s="366"/>
-      <c r="M6" s="366"/>
-      <c r="N6" s="366"/>
-      <c r="O6" s="366"/>
-      <c r="P6" s="366"/>
-      <c r="Q6" s="366"/>
-      <c r="R6" s="366"/>
+      <c r="F6" s="364"/>
+      <c r="G6" s="364"/>
+      <c r="H6" s="364"/>
+      <c r="I6" s="364"/>
+      <c r="J6" s="364"/>
+      <c r="K6" s="364"/>
+      <c r="L6" s="364"/>
+      <c r="M6" s="364"/>
+      <c r="N6" s="364"/>
+      <c r="O6" s="364"/>
+      <c r="P6" s="364"/>
+      <c r="Q6" s="364"/>
+      <c r="R6" s="364"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="363" t="s">
@@ -17072,21 +17072,21 @@
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="364" t="s">
+      <c r="H27" s="365" t="s">
         <v>95</v>
       </c>
-      <c r="I27" s="364"/>
-      <c r="J27" s="364"/>
-      <c r="K27" s="364"/>
-      <c r="L27" s="364"/>
-      <c r="M27" s="364"/>
-      <c r="N27" s="364"/>
-      <c r="O27" s="364"/>
-      <c r="P27" s="364"/>
-      <c r="Q27" s="364"/>
-      <c r="R27" s="364"/>
-      <c r="S27" s="364"/>
-      <c r="T27" s="364"/>
+      <c r="I27" s="365"/>
+      <c r="J27" s="365"/>
+      <c r="K27" s="365"/>
+      <c r="L27" s="365"/>
+      <c r="M27" s="365"/>
+      <c r="N27" s="365"/>
+      <c r="O27" s="365"/>
+      <c r="P27" s="365"/>
+      <c r="Q27" s="365"/>
+      <c r="R27" s="365"/>
+      <c r="S27" s="365"/>
+      <c r="T27" s="365"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
@@ -17402,21 +17402,21 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
-      <c r="F37" s="365" t="s">
+      <c r="F37" s="366" t="s">
         <v>99</v>
       </c>
-      <c r="G37" s="365"/>
-      <c r="H37" s="365"/>
-      <c r="I37" s="365"/>
-      <c r="J37" s="365"/>
-      <c r="K37" s="365"/>
-      <c r="L37" s="365"/>
-      <c r="M37" s="365"/>
-      <c r="N37" s="365"/>
-      <c r="O37" s="365"/>
-      <c r="P37" s="365"/>
-      <c r="Q37" s="365"/>
-      <c r="R37" s="365"/>
+      <c r="G37" s="366"/>
+      <c r="H37" s="366"/>
+      <c r="I37" s="366"/>
+      <c r="J37" s="366"/>
+      <c r="K37" s="366"/>
+      <c r="L37" s="366"/>
+      <c r="M37" s="366"/>
+      <c r="N37" s="366"/>
+      <c r="O37" s="366"/>
+      <c r="P37" s="366"/>
+      <c r="Q37" s="366"/>
+      <c r="R37" s="366"/>
     </row>
     <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="24" t="s">
@@ -17732,21 +17732,21 @@
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
-      <c r="F48" s="364" t="s">
+      <c r="F48" s="365" t="s">
         <v>101</v>
       </c>
-      <c r="G48" s="364"/>
-      <c r="H48" s="364"/>
-      <c r="I48" s="364"/>
-      <c r="J48" s="364"/>
-      <c r="K48" s="364"/>
-      <c r="L48" s="364"/>
-      <c r="M48" s="364"/>
-      <c r="N48" s="364"/>
-      <c r="O48" s="364"/>
-      <c r="P48" s="364"/>
-      <c r="Q48" s="364"/>
-      <c r="R48" s="364"/>
+      <c r="G48" s="365"/>
+      <c r="H48" s="365"/>
+      <c r="I48" s="365"/>
+      <c r="J48" s="365"/>
+      <c r="K48" s="365"/>
+      <c r="L48" s="365"/>
+      <c r="M48" s="365"/>
+      <c r="N48" s="365"/>
+      <c r="O48" s="365"/>
+      <c r="P48" s="365"/>
+      <c r="Q48" s="365"/>
+      <c r="R48" s="365"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
@@ -18058,12 +18058,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E6:R6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="H27:T27"/>
     <mergeCell ref="F37:R37"/>
@@ -18072,6 +18066,12 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E6:R6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -26151,7 +26151,7 @@
       <c r="D68" s="100"/>
       <c r="E68" s="218">
         <f>main!L82/1000</f>
-        <v>279.25</v>
+        <v>282.64999999999998</v>
       </c>
       <c r="F68" s="218">
         <f>main!M82/1000</f>
@@ -26159,7 +26159,7 @@
       </c>
       <c r="G68" s="151">
         <f>main!N82/1000</f>
-        <v>303.95100000000002</v>
+        <v>284.15100000000001</v>
       </c>
       <c r="H68" s="218">
         <f>main!O82/1000</f>
@@ -26417,7 +26417,7 @@
       </c>
       <c r="G71" s="150">
         <f t="shared" ref="G71:K71" si="118">G68-G69</f>
-        <v>0</v>
+        <v>-19.800000000000011</v>
       </c>
       <c r="H71" s="217">
         <f t="shared" si="118"/>
@@ -26648,7 +26648,7 @@
       </c>
       <c r="J2" s="102">
         <f>'add-ons calculations'!E68</f>
-        <v>279.25</v>
+        <v>282.64999999999998</v>
       </c>
       <c r="K2" s="102">
         <f>main!L$40/1000</f>
@@ -26760,11 +26760,11 @@
         <v>0.63599999999996726</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>-19.800000000000011</v>
       </c>
       <c r="J4" s="151">
         <f>'add-ons calculations'!G68</f>
-        <v>303.95100000000002</v>
+        <v>284.15100000000001</v>
       </c>
       <c r="K4" s="102">
         <f>main!N$40/1000</f>
@@ -31165,7 +31165,7 @@
         <v>0.63599999999996726</v>
       </c>
       <c r="I3" s="259">
-        <v>0</v>
+        <v>-19.800000000000011</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -32784,21 +32784,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA9F3DB0CD4D844B918872BCED9B9CF9" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61f75d9b13a46a58fd2456a565edcb9c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cac5d118-ba7b-4807-b700-df6f95cfff50" xmlns:ns3="66951ee6-cd93-49c7-9437-e871b2a117d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d86870d415110e2c98f3a885b29630d1" ns2:_="" ns3:_="">
     <xsd:import namespace="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
@@ -33015,10 +33000,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B484070-5C48-4F32-AF92-870650EA512F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
+    <ds:schemaRef ds:uri="66951ee6-cd93-49c7-9437-e871b2a117d6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -33041,20 +33052,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B484070-5C48-4F32-AF92-870650EA512F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
-    <ds:schemaRef ds:uri="66951ee6-cd93-49c7-9437-e871b2a117d6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>